<commit_message>
Updated April month tasks
</commit_message>
<xml_diff>
--- a/ATS Task List.xlsx
+++ b/ATS Task List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="283">
   <si>
     <t>Task</t>
   </si>
@@ -724,12 +724,207 @@
   <si>
     <t>Second Phase of AutoFollowUp module</t>
   </si>
+  <si>
+    <t>Mon 18-04-2022 20:03</t>
+  </si>
+  <si>
+    <t>Issue in Candidate id 154551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATS Issue : Need to fix on priority </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Issue with  Candidate “Nitin Kumar” and 64624 (Need to close this ticket) </t>
+  </si>
+  <si>
+    <t>Mon 18-04-2022 19:58</t>
+  </si>
+  <si>
+    <t>Issue with Opening Id 71519</t>
+  </si>
+  <si>
+    <t>Mon 18-04-2022 17:48</t>
+  </si>
+  <si>
+    <t>Issue with Opening Id 69333</t>
+  </si>
+  <si>
+    <t>Mon 18-04-2022 17:42</t>
+  </si>
+  <si>
+    <t>Required Server for WCF deployment</t>
+  </si>
+  <si>
+    <t>itsupport &lt;itsupport@chetu.com&gt;</t>
+  </si>
+  <si>
+    <t>Mon 18-04-2022 15:22</t>
+  </si>
+  <si>
+    <t>Requested for Deployement of Outlook PlugIn Service On QA environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to close </t>
+  </si>
+  <si>
+    <t>Thu 14-04-2022 20:47</t>
+  </si>
+  <si>
+    <t>Closed ticket no. 69752</t>
+  </si>
+  <si>
+    <t>ATS Issue : Candidate image not showing</t>
+  </si>
+  <si>
+    <t>Thu 14-04-2022 19:41</t>
+  </si>
+  <si>
+    <t>Issue with candidate id 156179</t>
+  </si>
+  <si>
+    <t>Mayank Rana</t>
+  </si>
+  <si>
+    <t>Wed 13-04-2022 23:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> added mayank rana in offer letter , and remove Sonali mishra2.</t>
+  </si>
+  <si>
+    <t>Mon 11-04-2022 21:20</t>
+  </si>
+  <si>
+    <t>Discussed on call</t>
+  </si>
+  <si>
+    <t>Generated CBT of Candidate id 145495</t>
+  </si>
+  <si>
+    <t>Need to check the access on review and other portals</t>
+  </si>
+  <si>
+    <t>gautamb@chetu.com</t>
+  </si>
+  <si>
+    <t>Fri 08-04-2022 20:01</t>
+  </si>
+  <si>
+    <t>Provided FM access</t>
+  </si>
+  <si>
+    <t>Assigned Ticket number – 71908 to Nishant Parihar , – 71910 to Shalini B .  </t>
+  </si>
+  <si>
+    <t>Unable to Assign Opening - 71908  &amp; 71910</t>
+  </si>
+  <si>
+    <t>Wed 06-04-2022 19:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unable to Offer Candidate - ATS Issue </t>
+  </si>
+  <si>
+    <t>Candidate id 155736-candidate (Kritesh) is showing in hiring portal with image but when I am going to offer his details is not showing</t>
+  </si>
+  <si>
+    <t>Tue 05-04-2022 16:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Able to Save Data </t>
+  </si>
+  <si>
+    <t>Friday, April 1, 2022 7:37 AM</t>
+  </si>
+  <si>
+    <t>Mon 04-04-2022 20:18</t>
+  </si>
+  <si>
+    <t>issue in Hiring.chetu.com</t>
+  </si>
+  <si>
+    <t>Isse in Opening ID-  68696</t>
+  </si>
+  <si>
+    <t>Mon 04-04-2022 20:07</t>
+  </si>
+  <si>
+    <t>Opening ID</t>
+  </si>
+  <si>
+    <t>remove Sumit Sharma from ATS offer letter access. And add Anuj Garg3</t>
+  </si>
+  <si>
+    <t>Mon 04-04-2022 18:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sumit Sharma </t>
+  </si>
+  <si>
+    <t>Resource Id - 70200</t>
+  </si>
+  <si>
+    <t>Wed 30-03-2022 23:01</t>
+  </si>
+  <si>
+    <t>ATS Issue !</t>
+  </si>
+  <si>
+    <t>Wed 30-03-2022 16:20</t>
+  </si>
+  <si>
+    <t>Issue with candidate Pradhap Palani</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5 hour</t>
+  </si>
+  <si>
+    <t>tarung@chetu.com</t>
+  </si>
+  <si>
+    <t>CBT Status</t>
+  </si>
+  <si>
+    <t>Wed 30-03-2022 15:52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolved issue of Candidate name Govind., it’s showing “NO” in CBT Pass Section however he passed in CBT </t>
+  </si>
+  <si>
+    <t>Candidate not linking | ATS issue</t>
+  </si>
+  <si>
+    <t>jhalakk@chetu.com</t>
+  </si>
+  <si>
+    <t>Wed 23-03-2022 20:25</t>
+  </si>
+  <si>
+    <t>Opening ID 71792 issue</t>
+  </si>
+  <si>
+    <t>#70056</t>
+  </si>
+  <si>
+    <t>Wed 23-03-2022 22:55</t>
+  </si>
+  <si>
+    <t>Hiring Portal result Required !</t>
+  </si>
+  <si>
+    <t>Wed 27-04-2022 15:08</t>
+  </si>
+  <si>
+    <t>Wed 27-04-2022 17:30</t>
+  </si>
+  <si>
+    <t>unable to find his CBT Result on portal with Emp Id 9042</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -808,6 +1003,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -916,7 +1129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -969,17 +1182,36 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1261,10 +1493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ70"/>
+  <dimension ref="A1:AQ110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,12 +1572,12 @@
       <c r="AQ1" s="15"/>
     </row>
     <row r="2" spans="1:43" s="2" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="40">
+      <c r="A2" s="43">
         <v>44501</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
       <c r="F2" s="22"/>
       <c r="G2" s="18"/>
       <c r="H2" s="29"/>
@@ -1809,12 +2041,12 @@
       <c r="AQ10" s="15"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="40">
+      <c r="A11" s="43">
         <v>44531</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
       <c r="F11" s="22"/>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
@@ -2520,12 +2752,12 @@
       <c r="AQ24" s="15"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A25" s="40">
+      <c r="A25" s="43">
         <v>44562</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
       <c r="F25" s="22"/>
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
@@ -2949,12 +3181,12 @@
       <c r="AQ32" s="15"/>
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="40">
+      <c r="A33" s="43">
         <v>44593</v>
       </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
       <c r="F33" s="22"/>
       <c r="G33" s="18"/>
       <c r="H33" s="18"/>
@@ -3215,7 +3447,7 @@
       <c r="E46" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="F46" s="41" t="s">
+      <c r="F46" s="44" t="s">
         <v>114</v>
       </c>
     </row>
@@ -3235,7 +3467,7 @@
       <c r="E47" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="F47" s="41"/>
+      <c r="F47" s="44"/>
       <c r="G47" s="18"/>
       <c r="H47" s="18"/>
       <c r="I47" s="18"/>
@@ -3274,72 +3506,98 @@
       <c r="AP47" s="17"/>
       <c r="AQ47" s="17"/>
     </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C48" t="s">
-        <v>160</v>
-      </c>
-      <c r="D48" t="s">
-        <v>161</v>
-      </c>
-      <c r="F48" s="24" t="s">
-        <v>162</v>
-      </c>
+    <row r="48" spans="1:43" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A48" s="43">
+        <v>44621</v>
+      </c>
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="18"/>
+      <c r="R48" s="18"/>
+      <c r="S48" s="18"/>
+      <c r="T48" s="18"/>
+      <c r="U48" s="18"/>
+      <c r="V48" s="18"/>
+      <c r="W48" s="18"/>
+      <c r="X48" s="18"/>
+      <c r="Y48" s="18"/>
+      <c r="Z48" s="16"/>
+      <c r="AA48" s="16"/>
+      <c r="AB48" s="16"/>
+      <c r="AC48" s="16"/>
+      <c r="AD48" s="16"/>
+      <c r="AE48" s="16"/>
+      <c r="AF48" s="16"/>
+      <c r="AG48" s="16"/>
+      <c r="AH48" s="16"/>
+      <c r="AI48" s="16"/>
+      <c r="AJ48" s="16"/>
+      <c r="AK48" s="16"/>
+      <c r="AL48" s="16"/>
+      <c r="AM48" s="16"/>
+      <c r="AN48" s="16"/>
+      <c r="AO48" s="16"/>
+      <c r="AP48" s="16"/>
+      <c r="AQ48" s="16"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>110</v>
+        <v>159</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="4">
-        <v>44624.019444444442</v>
+        <v>90</v>
+      </c>
+      <c r="C49" t="s">
+        <v>160</v>
       </c>
       <c r="D49" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>116</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>167</v>
+        <v>110</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="C50" s="4">
-        <v>44624.978472222225</v>
+        <v>44624.019444444442</v>
       </c>
       <c r="D50" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C51" t="s">
-        <v>168</v>
+        <v>90</v>
+      </c>
+      <c r="C51" s="4">
+        <v>44624.978472222225</v>
       </c>
       <c r="D51" t="s">
-        <v>169</v>
-      </c>
-      <c r="E51" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F51" s="24" t="s">
         <v>135</v>
@@ -3347,19 +3605,19 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>63</v>
+        <v>170</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C52" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D52" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E52" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F52" s="24" t="s">
         <v>135</v>
@@ -3367,95 +3625,95 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>176</v>
+        <v>63</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C53" s="4">
-        <v>44630.90625</v>
+        <v>9</v>
+      </c>
+      <c r="C53" t="s">
+        <v>172</v>
       </c>
       <c r="D53" t="s">
-        <v>175</v>
+        <v>173</v>
+      </c>
+      <c r="E53" t="s">
+        <v>174</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" t="s">
-        <v>178</v>
+        <v>90</v>
+      </c>
+      <c r="C54" s="4">
+        <v>44630.90625</v>
       </c>
       <c r="D54" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>181</v>
+        <v>178</v>
+      </c>
+      <c r="D55" t="s">
+        <v>179</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>194</v>
-      </c>
-      <c r="D58" t="s">
-        <v>195</v>
-      </c>
-      <c r="E58" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="F58" s="24" t="s">
         <v>135</v>
@@ -3463,199 +3721,1393 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C59" s="4">
-        <v>44637.89166666667</v>
+      <c r="C59" t="s">
+        <v>194</v>
       </c>
       <c r="D59" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E59" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>200</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C60" t="s">
-        <v>188</v>
+      <c r="C60" s="4">
+        <v>44637.89166666667</v>
+      </c>
+      <c r="D60" t="s">
+        <v>198</v>
       </c>
       <c r="E60" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>135</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" t="s">
+        <v>188</v>
+      </c>
+      <c r="E61" t="s">
+        <v>189</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C61" s="4">
+      <c r="C62" s="4">
         <v>44642.008333333331</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>192</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E62" t="s">
         <v>191</v>
       </c>
-      <c r="F61" s="24" t="s">
+      <c r="F62" s="24" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="4"/>
-    </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C63" s="4"/>
+      <c r="A63" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="B63" s="48" t="s">
+        <v>274</v>
+      </c>
+      <c r="C63" s="49">
+        <v>44643.805555555555</v>
+      </c>
+      <c r="D63" s="47" t="s">
+        <v>275</v>
+      </c>
+      <c r="E63" s="47" t="s">
+        <v>276</v>
+      </c>
+      <c r="F63" s="50" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="B64" s="37"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38" t="s">
-        <v>216</v>
-      </c>
-      <c r="E64" s="38" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="47" t="s">
+        <v>277</v>
+      </c>
+      <c r="B64" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" s="49">
+        <v>44643.936805555553</v>
+      </c>
+      <c r="D64" s="47" t="s">
+        <v>278</v>
+      </c>
+      <c r="E64" s="51"/>
+      <c r="F64" s="50" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>63</v>
+        <v>270</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>103</v>
+        <v>269</v>
       </c>
       <c r="C65" s="4">
-        <v>44670.671527777777</v>
+        <v>44649.828472222223</v>
       </c>
       <c r="D65" t="s">
-        <v>214</v>
-      </c>
-      <c r="E65" s="44" t="s">
-        <v>215</v>
+        <v>271</v>
+      </c>
+      <c r="E65" t="s">
+        <v>272</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="s">
-        <v>63</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>265</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C66" s="4">
-        <v>44671.679166666669</v>
+        <v>44648.92083333333</v>
       </c>
       <c r="D66" t="s">
-        <v>212</v>
+        <v>266</v>
       </c>
       <c r="E66" t="s">
-        <v>213</v>
+        <v>267</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="67" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>210</v>
+        <v>263</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C67" s="4">
-        <v>44671.828472222223</v>
+        <v>44650.872916666667</v>
       </c>
       <c r="D67" t="s">
-        <v>211</v>
+        <v>264</v>
       </c>
       <c r="F67" s="24" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="68" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="C68" s="4"/>
+    </row>
+    <row r="69" spans="1:43" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A69" s="43">
+        <v>44652</v>
+      </c>
+      <c r="B69" s="43"/>
+      <c r="C69" s="43"/>
+      <c r="D69" s="43"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="22"/>
+    </row>
+    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A70"/>
+      <c r="B70"/>
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A71"/>
+      <c r="B71"/>
+      <c r="F71"/>
+    </row>
+    <row r="72" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>262</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" s="4">
+        <v>44655.722222222219</v>
+      </c>
+      <c r="D72" t="s">
+        <v>261</v>
+      </c>
+      <c r="E72" t="s">
+        <v>260</v>
+      </c>
+      <c r="F72" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="73" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>259</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C73" s="4">
+        <v>44655.751388888886</v>
+      </c>
+      <c r="D73" t="s">
+        <v>258</v>
+      </c>
+      <c r="E73" t="s">
+        <v>257</v>
+      </c>
+      <c r="F73" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>253</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C74" t="s">
+        <v>254</v>
+      </c>
+      <c r="D74" t="s">
+        <v>255</v>
+      </c>
+      <c r="E74" t="s">
+        <v>256</v>
+      </c>
+      <c r="F74" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="75" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>250</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C75" s="4">
+        <v>44656.659722222219</v>
+      </c>
+      <c r="D75" t="s">
+        <v>252</v>
+      </c>
+      <c r="E75" t="s">
+        <v>251</v>
+      </c>
+      <c r="F75" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="76" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>248</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" s="4">
+        <v>44657.71875</v>
+      </c>
+      <c r="D76" t="s">
+        <v>249</v>
+      </c>
+      <c r="E76" t="s">
+        <v>247</v>
+      </c>
+      <c r="F76" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>243</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C77" s="4">
+        <v>44657.767361111109</v>
+      </c>
+      <c r="D77" t="s">
+        <v>245</v>
+      </c>
+      <c r="E77" t="s">
+        <v>246</v>
+      </c>
+      <c r="F77" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>110</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C78" t="s">
+        <v>241</v>
+      </c>
+      <c r="D78" t="s">
+        <v>240</v>
+      </c>
+      <c r="E78" t="s">
+        <v>242</v>
+      </c>
+      <c r="F78" t="s">
+        <v>200</v>
+      </c>
+      <c r="G78" s="18"/>
+      <c r="H78" s="18"/>
+      <c r="I78" s="18"/>
+      <c r="J78" s="18"/>
+      <c r="K78" s="18"/>
+      <c r="L78" s="18"/>
+      <c r="M78" s="18"/>
+      <c r="N78" s="18"/>
+      <c r="O78" s="18"/>
+      <c r="P78" s="18"/>
+      <c r="Q78" s="18"/>
+      <c r="R78" s="18"/>
+      <c r="S78" s="18"/>
+      <c r="T78" s="18"/>
+      <c r="U78" s="18"/>
+      <c r="V78" s="18"/>
+      <c r="W78" s="18"/>
+      <c r="X78" s="18"/>
+      <c r="Y78" s="18"/>
+      <c r="Z78" s="16"/>
+      <c r="AA78" s="16"/>
+      <c r="AB78" s="16"/>
+      <c r="AC78" s="16"/>
+      <c r="AD78" s="16"/>
+      <c r="AE78" s="16"/>
+      <c r="AF78" s="16"/>
+      <c r="AG78" s="16"/>
+      <c r="AH78" s="16"/>
+      <c r="AI78" s="16"/>
+      <c r="AJ78" s="16"/>
+      <c r="AK78" s="16"/>
+      <c r="AL78" s="16"/>
+      <c r="AM78" s="16"/>
+      <c r="AN78" s="16"/>
+      <c r="AO78" s="16"/>
+      <c r="AP78" s="16"/>
+      <c r="AQ78" s="16"/>
+    </row>
+    <row r="79" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>237</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" s="4">
+        <v>44664.931250000001</v>
+      </c>
+      <c r="D79" t="s">
+        <v>238</v>
+      </c>
+      <c r="E79" s="45" t="s">
+        <v>239</v>
+      </c>
+      <c r="F79" t="s">
+        <v>200</v>
+      </c>
+      <c r="G79" s="18"/>
+      <c r="H79" s="18"/>
+      <c r="I79" s="18"/>
+      <c r="J79" s="18"/>
+      <c r="K79" s="18"/>
+      <c r="L79" s="18"/>
+      <c r="M79" s="18"/>
+      <c r="N79" s="18"/>
+      <c r="O79" s="18"/>
+      <c r="P79" s="18"/>
+      <c r="Q79" s="18"/>
+      <c r="R79" s="18"/>
+      <c r="S79" s="18"/>
+      <c r="T79" s="18"/>
+      <c r="U79" s="18"/>
+      <c r="V79" s="18"/>
+      <c r="W79" s="18"/>
+      <c r="X79" s="18"/>
+      <c r="Y79" s="18"/>
+      <c r="Z79" s="16"/>
+      <c r="AA79" s="16"/>
+      <c r="AB79" s="16"/>
+      <c r="AC79" s="16"/>
+      <c r="AD79" s="16"/>
+      <c r="AE79" s="16"/>
+      <c r="AF79" s="16"/>
+      <c r="AG79" s="16"/>
+      <c r="AH79" s="16"/>
+      <c r="AI79" s="16"/>
+      <c r="AJ79" s="16"/>
+      <c r="AK79" s="16"/>
+      <c r="AL79" s="16"/>
+      <c r="AM79" s="16"/>
+      <c r="AN79" s="16"/>
+      <c r="AO79" s="16"/>
+      <c r="AP79" s="16"/>
+      <c r="AQ79" s="16"/>
+    </row>
+    <row r="80" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>234</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C80" s="4">
+        <v>44665.634722222225</v>
+      </c>
+      <c r="D80" t="s">
+        <v>235</v>
+      </c>
+      <c r="E80" t="s">
+        <v>236</v>
+      </c>
+      <c r="F80" t="s">
+        <v>200</v>
+      </c>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+      <c r="I80" s="18"/>
+      <c r="J80" s="18"/>
+      <c r="K80" s="18"/>
+      <c r="L80" s="18"/>
+      <c r="M80" s="18"/>
+      <c r="N80" s="18"/>
+      <c r="O80" s="18"/>
+      <c r="P80" s="18"/>
+      <c r="Q80" s="18"/>
+      <c r="R80" s="18"/>
+      <c r="S80" s="18"/>
+      <c r="T80" s="18"/>
+      <c r="U80" s="18"/>
+      <c r="V80" s="18"/>
+      <c r="W80" s="18"/>
+      <c r="X80" s="18"/>
+      <c r="Y80" s="18"/>
+      <c r="Z80" s="16"/>
+      <c r="AA80" s="16"/>
+      <c r="AB80" s="16"/>
+      <c r="AC80" s="16"/>
+      <c r="AD80" s="16"/>
+      <c r="AE80" s="16"/>
+      <c r="AF80" s="16"/>
+      <c r="AG80" s="16"/>
+      <c r="AH80" s="16"/>
+      <c r="AI80" s="16"/>
+      <c r="AJ80" s="16"/>
+      <c r="AK80" s="16"/>
+      <c r="AL80" s="16"/>
+      <c r="AM80" s="16"/>
+      <c r="AN80" s="16"/>
+      <c r="AO80" s="16"/>
+      <c r="AP80" s="16"/>
+      <c r="AQ80" s="16"/>
+    </row>
+    <row r="81" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>231</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" s="4">
+        <v>44662.710416666669</v>
+      </c>
+      <c r="D81" t="s">
+        <v>232</v>
+      </c>
+      <c r="E81" t="s">
+        <v>233</v>
+      </c>
+      <c r="F81" t="s">
+        <v>200</v>
+      </c>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="18"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="18"/>
+      <c r="L81" s="18"/>
+      <c r="M81" s="18"/>
+      <c r="N81" s="18"/>
+      <c r="O81" s="18"/>
+      <c r="P81" s="18"/>
+      <c r="Q81" s="18"/>
+      <c r="R81" s="18"/>
+      <c r="S81" s="18"/>
+      <c r="T81" s="18"/>
+      <c r="U81" s="18"/>
+      <c r="V81" s="18"/>
+      <c r="W81" s="18"/>
+      <c r="X81" s="18"/>
+      <c r="Y81" s="18"/>
+      <c r="Z81" s="16"/>
+      <c r="AA81" s="16"/>
+      <c r="AB81" s="16"/>
+      <c r="AC81" s="16"/>
+      <c r="AD81" s="16"/>
+      <c r="AE81" s="16"/>
+      <c r="AF81" s="16"/>
+      <c r="AG81" s="16"/>
+      <c r="AH81" s="16"/>
+      <c r="AI81" s="16"/>
+      <c r="AJ81" s="16"/>
+      <c r="AK81" s="16"/>
+      <c r="AL81" s="16"/>
+      <c r="AM81" s="16"/>
+      <c r="AN81" s="16"/>
+      <c r="AO81" s="16"/>
+      <c r="AP81" s="16"/>
+      <c r="AQ81" s="16"/>
+    </row>
+    <row r="82" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>227</v>
+      </c>
+      <c r="B82" t="s">
+        <v>228</v>
+      </c>
+      <c r="C82" s="4">
+        <v>44664.661111111112</v>
+      </c>
+      <c r="D82" t="s">
+        <v>229</v>
+      </c>
+      <c r="E82" t="s">
+        <v>230</v>
+      </c>
+      <c r="F82"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
+      <c r="I82" s="18"/>
+      <c r="J82" s="18"/>
+      <c r="K82" s="18"/>
+      <c r="L82" s="18"/>
+      <c r="M82" s="18"/>
+      <c r="N82" s="18"/>
+      <c r="O82" s="18"/>
+      <c r="P82" s="18"/>
+      <c r="Q82" s="18"/>
+      <c r="R82" s="18"/>
+      <c r="S82" s="18"/>
+      <c r="T82" s="18"/>
+      <c r="U82" s="18"/>
+      <c r="V82" s="18"/>
+      <c r="W82" s="18"/>
+      <c r="X82" s="18"/>
+      <c r="Y82" s="18"/>
+      <c r="Z82" s="16"/>
+      <c r="AA82" s="16"/>
+      <c r="AB82" s="16"/>
+      <c r="AC82" s="16"/>
+      <c r="AD82" s="16"/>
+      <c r="AE82" s="16"/>
+      <c r="AF82" s="16"/>
+      <c r="AG82" s="16"/>
+      <c r="AH82" s="16"/>
+      <c r="AI82" s="16"/>
+      <c r="AJ82" s="16"/>
+      <c r="AK82" s="16"/>
+      <c r="AL82" s="16"/>
+      <c r="AM82" s="16"/>
+      <c r="AN82" s="16"/>
+      <c r="AO82" s="16"/>
+      <c r="AP82" s="16"/>
+      <c r="AQ82" s="16"/>
+    </row>
+    <row r="83" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>63</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B83" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C68" s="4">
+      <c r="C83" s="4">
+        <v>44669.722916666666</v>
+      </c>
+      <c r="D83" t="s">
+        <v>226</v>
+      </c>
+      <c r="E83" t="s">
+        <v>225</v>
+      </c>
+      <c r="F83" t="s">
+        <v>200</v>
+      </c>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+      <c r="J83" s="18"/>
+      <c r="K83" s="18"/>
+      <c r="L83" s="18"/>
+      <c r="M83" s="18"/>
+      <c r="N83" s="18"/>
+      <c r="O83" s="18"/>
+      <c r="P83" s="18"/>
+      <c r="Q83" s="18"/>
+      <c r="R83" s="18"/>
+      <c r="S83" s="18"/>
+      <c r="T83" s="18"/>
+      <c r="U83" s="18"/>
+      <c r="V83" s="18"/>
+      <c r="W83" s="18"/>
+      <c r="X83" s="18"/>
+      <c r="Y83" s="18"/>
+      <c r="Z83" s="16"/>
+      <c r="AA83" s="16"/>
+      <c r="AB83" s="16"/>
+      <c r="AC83" s="16"/>
+      <c r="AD83" s="16"/>
+      <c r="AE83" s="16"/>
+      <c r="AF83" s="16"/>
+      <c r="AG83" s="16"/>
+      <c r="AH83" s="16"/>
+      <c r="AI83" s="16"/>
+      <c r="AJ83" s="16"/>
+      <c r="AK83" s="16"/>
+      <c r="AL83" s="16"/>
+      <c r="AM83" s="16"/>
+      <c r="AN83" s="16"/>
+      <c r="AO83" s="16"/>
+      <c r="AP83" s="16"/>
+      <c r="AQ83" s="16"/>
+    </row>
+    <row r="84" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>63</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C84" s="4">
+        <v>44667.622916666667</v>
+      </c>
+      <c r="D84" t="s">
+        <v>224</v>
+      </c>
+      <c r="E84" t="s">
+        <v>223</v>
+      </c>
+      <c r="F84" t="s">
+        <v>200</v>
+      </c>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
+      <c r="J84" s="18"/>
+      <c r="K84" s="18"/>
+      <c r="L84" s="18"/>
+      <c r="M84" s="18"/>
+      <c r="N84" s="18"/>
+      <c r="O84" s="18"/>
+      <c r="P84" s="18"/>
+      <c r="Q84" s="18"/>
+      <c r="R84" s="18"/>
+      <c r="S84" s="18"/>
+      <c r="T84" s="18"/>
+      <c r="U84" s="18"/>
+      <c r="V84" s="18"/>
+      <c r="W84" s="18"/>
+      <c r="X84" s="18"/>
+      <c r="Y84" s="18"/>
+      <c r="Z84" s="16"/>
+      <c r="AA84" s="16"/>
+      <c r="AB84" s="16"/>
+      <c r="AC84" s="16"/>
+      <c r="AD84" s="16"/>
+      <c r="AE84" s="16"/>
+      <c r="AF84" s="16"/>
+      <c r="AG84" s="16"/>
+      <c r="AH84" s="16"/>
+      <c r="AI84" s="16"/>
+      <c r="AJ84" s="16"/>
+      <c r="AK84" s="16"/>
+      <c r="AL84" s="16"/>
+      <c r="AM84" s="16"/>
+      <c r="AN84" s="16"/>
+      <c r="AO84" s="16"/>
+      <c r="AP84" s="16"/>
+      <c r="AQ84" s="16"/>
+    </row>
+    <row r="85" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>220</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C85" s="4">
+        <v>44667.89166666667</v>
+      </c>
+      <c r="D85" t="s">
+        <v>222</v>
+      </c>
+      <c r="E85" t="s">
+        <v>221</v>
+      </c>
+      <c r="F85" t="s">
+        <v>112</v>
+      </c>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
+      <c r="I85" s="18"/>
+      <c r="J85" s="18"/>
+      <c r="K85" s="18"/>
+      <c r="L85" s="18"/>
+      <c r="M85" s="18"/>
+      <c r="N85" s="18"/>
+      <c r="O85" s="18"/>
+      <c r="P85" s="18"/>
+      <c r="Q85" s="18"/>
+      <c r="R85" s="18"/>
+      <c r="S85" s="18"/>
+      <c r="T85" s="18"/>
+      <c r="U85" s="18"/>
+      <c r="V85" s="18"/>
+      <c r="W85" s="18"/>
+      <c r="X85" s="18"/>
+      <c r="Y85" s="18"/>
+      <c r="Z85" s="16"/>
+      <c r="AA85" s="16"/>
+      <c r="AB85" s="16"/>
+      <c r="AC85" s="16"/>
+      <c r="AD85" s="16"/>
+      <c r="AE85" s="16"/>
+      <c r="AF85" s="16"/>
+      <c r="AG85" s="16"/>
+      <c r="AH85" s="16"/>
+      <c r="AI85" s="16"/>
+      <c r="AJ85" s="16"/>
+      <c r="AK85" s="16"/>
+      <c r="AL85" s="16"/>
+      <c r="AM85" s="16"/>
+      <c r="AN85" s="16"/>
+      <c r="AO85" s="16"/>
+      <c r="AP85" s="16"/>
+      <c r="AQ85" s="16"/>
+    </row>
+    <row r="86" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>63</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C86" s="4">
+        <v>44667.822222222225</v>
+      </c>
+      <c r="D86" t="s">
+        <v>218</v>
+      </c>
+      <c r="E86" t="s">
+        <v>219</v>
+      </c>
+      <c r="F86" t="s">
+        <v>200</v>
+      </c>
+      <c r="G86" s="18"/>
+      <c r="H86" s="18"/>
+      <c r="I86" s="18"/>
+      <c r="J86" s="18"/>
+      <c r="K86" s="18"/>
+      <c r="L86" s="18"/>
+      <c r="M86" s="18"/>
+      <c r="N86" s="18"/>
+      <c r="O86" s="18"/>
+      <c r="P86" s="18"/>
+      <c r="Q86" s="18"/>
+      <c r="R86" s="18"/>
+      <c r="S86" s="18"/>
+      <c r="T86" s="18"/>
+      <c r="U86" s="18"/>
+      <c r="V86" s="18"/>
+      <c r="W86" s="18"/>
+      <c r="X86" s="18"/>
+      <c r="Y86" s="18"/>
+      <c r="Z86" s="16"/>
+      <c r="AA86" s="16"/>
+      <c r="AB86" s="16"/>
+      <c r="AC86" s="16"/>
+      <c r="AD86" s="16"/>
+      <c r="AE86" s="16"/>
+      <c r="AF86" s="16"/>
+      <c r="AG86" s="16"/>
+      <c r="AH86" s="16"/>
+      <c r="AI86" s="16"/>
+      <c r="AJ86" s="16"/>
+      <c r="AK86" s="16"/>
+      <c r="AL86" s="16"/>
+      <c r="AM86" s="16"/>
+      <c r="AN86" s="16"/>
+      <c r="AO86" s="16"/>
+      <c r="AP86" s="16"/>
+      <c r="AQ86" s="16"/>
+    </row>
+    <row r="87" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="B87" s="37"/>
+      <c r="C87" s="38"/>
+      <c r="D87" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="E87" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="F87" s="24"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="18"/>
+      <c r="I87" s="18"/>
+      <c r="J87" s="18"/>
+      <c r="K87" s="18"/>
+      <c r="L87" s="18"/>
+      <c r="M87" s="18"/>
+      <c r="N87" s="18"/>
+      <c r="O87" s="18"/>
+      <c r="P87" s="18"/>
+      <c r="Q87" s="18"/>
+      <c r="R87" s="18"/>
+      <c r="S87" s="18"/>
+      <c r="T87" s="18"/>
+      <c r="U87" s="18"/>
+      <c r="V87" s="18"/>
+      <c r="W87" s="18"/>
+      <c r="X87" s="18"/>
+      <c r="Y87" s="18"/>
+      <c r="Z87" s="16"/>
+      <c r="AA87" s="16"/>
+      <c r="AB87" s="16"/>
+      <c r="AC87" s="16"/>
+      <c r="AD87" s="16"/>
+      <c r="AE87" s="16"/>
+      <c r="AF87" s="16"/>
+      <c r="AG87" s="16"/>
+      <c r="AH87" s="16"/>
+      <c r="AI87" s="16"/>
+      <c r="AJ87" s="16"/>
+      <c r="AK87" s="16"/>
+      <c r="AL87" s="16"/>
+      <c r="AM87" s="16"/>
+      <c r="AN87" s="16"/>
+      <c r="AO87" s="16"/>
+      <c r="AP87" s="16"/>
+      <c r="AQ87" s="16"/>
+    </row>
+    <row r="88" spans="1:43" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C88" s="4">
+        <v>44670.671527777777</v>
+      </c>
+      <c r="D88" t="s">
+        <v>214</v>
+      </c>
+      <c r="E88" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="F88" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="G88" s="18"/>
+      <c r="H88" s="18"/>
+      <c r="I88" s="18"/>
+      <c r="J88" s="18"/>
+      <c r="K88" s="18"/>
+      <c r="L88" s="18"/>
+      <c r="M88" s="18"/>
+      <c r="N88" s="18"/>
+      <c r="O88" s="18"/>
+      <c r="P88" s="18"/>
+      <c r="Q88" s="18"/>
+      <c r="R88" s="18"/>
+      <c r="S88" s="18"/>
+      <c r="T88" s="18"/>
+      <c r="U88" s="18"/>
+      <c r="V88" s="18"/>
+      <c r="W88" s="18"/>
+      <c r="X88" s="18"/>
+      <c r="Y88" s="18"/>
+      <c r="Z88" s="16"/>
+      <c r="AA88" s="16"/>
+      <c r="AB88" s="16"/>
+      <c r="AC88" s="16"/>
+      <c r="AD88" s="16"/>
+      <c r="AE88" s="16"/>
+      <c r="AF88" s="16"/>
+      <c r="AG88" s="16"/>
+      <c r="AH88" s="16"/>
+      <c r="AI88" s="16"/>
+      <c r="AJ88" s="16"/>
+      <c r="AK88" s="16"/>
+      <c r="AL88" s="16"/>
+      <c r="AM88" s="16"/>
+      <c r="AN88" s="16"/>
+      <c r="AO88" s="16"/>
+      <c r="AP88" s="16"/>
+      <c r="AQ88" s="16"/>
+    </row>
+    <row r="89" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C89" s="4">
+        <v>44671.679166666669</v>
+      </c>
+      <c r="D89" t="s">
+        <v>212</v>
+      </c>
+      <c r="E89" t="s">
+        <v>213</v>
+      </c>
+      <c r="F89" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="G89" s="18"/>
+      <c r="H89" s="18"/>
+      <c r="I89" s="18"/>
+      <c r="J89" s="18"/>
+      <c r="K89" s="18"/>
+      <c r="L89" s="18"/>
+      <c r="M89" s="18"/>
+      <c r="N89" s="18"/>
+      <c r="O89" s="18"/>
+      <c r="P89" s="18"/>
+      <c r="Q89" s="18"/>
+      <c r="R89" s="18"/>
+      <c r="S89" s="18"/>
+      <c r="T89" s="18"/>
+      <c r="U89" s="18"/>
+      <c r="V89" s="18"/>
+      <c r="W89" s="18"/>
+      <c r="X89" s="18"/>
+      <c r="Y89" s="18"/>
+      <c r="Z89" s="16"/>
+      <c r="AA89" s="16"/>
+      <c r="AB89" s="16"/>
+      <c r="AC89" s="16"/>
+      <c r="AD89" s="16"/>
+      <c r="AE89" s="16"/>
+      <c r="AF89" s="16"/>
+      <c r="AG89" s="16"/>
+      <c r="AH89" s="16"/>
+      <c r="AI89" s="16"/>
+      <c r="AJ89" s="16"/>
+      <c r="AK89" s="16"/>
+      <c r="AL89" s="16"/>
+      <c r="AM89" s="16"/>
+      <c r="AN89" s="16"/>
+      <c r="AO89" s="16"/>
+      <c r="AP89" s="16"/>
+      <c r="AQ89" s="16"/>
+    </row>
+    <row r="90" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C90" s="4">
+        <v>44671.828472222223</v>
+      </c>
+      <c r="D90" t="s">
+        <v>211</v>
+      </c>
+      <c r="E90"/>
+      <c r="F90" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
+      <c r="J90" s="18"/>
+      <c r="K90" s="18"/>
+      <c r="L90" s="18"/>
+      <c r="M90" s="18"/>
+      <c r="N90" s="18"/>
+      <c r="O90" s="18"/>
+      <c r="P90" s="18"/>
+      <c r="Q90" s="18"/>
+      <c r="R90" s="18"/>
+      <c r="S90" s="18"/>
+      <c r="T90" s="18"/>
+      <c r="U90" s="18"/>
+      <c r="V90" s="18"/>
+      <c r="W90" s="18"/>
+      <c r="X90" s="18"/>
+      <c r="Y90" s="18"/>
+      <c r="Z90" s="16"/>
+      <c r="AA90" s="16"/>
+      <c r="AB90" s="16"/>
+      <c r="AC90" s="16"/>
+      <c r="AD90" s="16"/>
+      <c r="AE90" s="16"/>
+      <c r="AF90" s="16"/>
+      <c r="AG90" s="16"/>
+      <c r="AH90" s="16"/>
+      <c r="AI90" s="16"/>
+      <c r="AJ90" s="16"/>
+      <c r="AK90" s="16"/>
+      <c r="AL90" s="16"/>
+      <c r="AM90" s="16"/>
+      <c r="AN90" s="16"/>
+      <c r="AO90" s="16"/>
+      <c r="AP90" s="16"/>
+      <c r="AQ90" s="16"/>
+    </row>
+    <row r="91" spans="1:43" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>63</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C91" s="4">
         <v>44673.776388888888</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D91" t="s">
         <v>208</v>
       </c>
-      <c r="E68" s="43" t="s">
+      <c r="E91" s="41" t="s">
         <v>209</v>
       </c>
-      <c r="F68" s="24" t="s">
+      <c r="F91" s="24" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="13" t="s">
+      <c r="G91" s="18"/>
+      <c r="H91" s="18"/>
+      <c r="I91" s="18"/>
+      <c r="J91" s="18"/>
+      <c r="K91" s="18"/>
+      <c r="L91" s="18"/>
+      <c r="M91" s="18"/>
+      <c r="N91" s="18"/>
+      <c r="O91" s="18"/>
+      <c r="P91" s="18"/>
+      <c r="Q91" s="18"/>
+      <c r="R91" s="18"/>
+      <c r="S91" s="18"/>
+      <c r="T91" s="18"/>
+      <c r="U91" s="18"/>
+      <c r="V91" s="18"/>
+      <c r="W91" s="18"/>
+      <c r="X91" s="18"/>
+      <c r="Y91" s="18"/>
+      <c r="Z91" s="16"/>
+      <c r="AA91" s="16"/>
+      <c r="AB91" s="16"/>
+      <c r="AC91" s="16"/>
+      <c r="AD91" s="16"/>
+      <c r="AE91" s="16"/>
+      <c r="AF91" s="16"/>
+      <c r="AG91" s="16"/>
+      <c r="AH91" s="16"/>
+      <c r="AI91" s="16"/>
+      <c r="AJ91" s="16"/>
+      <c r="AK91" s="16"/>
+      <c r="AL91" s="16"/>
+      <c r="AM91" s="16"/>
+      <c r="AN91" s="16"/>
+      <c r="AO91" s="16"/>
+      <c r="AP91" s="16"/>
+      <c r="AQ91" s="16"/>
+    </row>
+    <row r="92" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B92" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C92" t="s">
         <v>204</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D92" t="s">
         <v>206</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E92" t="s">
         <v>207</v>
       </c>
-      <c r="F69" s="24" t="s">
+      <c r="F92" s="24" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="13" t="s">
+      <c r="G92" s="18"/>
+      <c r="H92" s="18"/>
+      <c r="I92" s="18"/>
+      <c r="J92" s="18"/>
+      <c r="K92" s="18"/>
+      <c r="L92" s="18"/>
+      <c r="M92" s="18"/>
+      <c r="N92" s="18"/>
+      <c r="O92" s="18"/>
+      <c r="P92" s="18"/>
+      <c r="Q92" s="18"/>
+      <c r="R92" s="18"/>
+      <c r="S92" s="18"/>
+      <c r="T92" s="18"/>
+      <c r="U92" s="18"/>
+      <c r="V92" s="18"/>
+      <c r="W92" s="18"/>
+      <c r="X92" s="18"/>
+      <c r="Y92" s="18"/>
+      <c r="Z92" s="16"/>
+      <c r="AA92" s="16"/>
+      <c r="AB92" s="16"/>
+      <c r="AC92" s="16"/>
+      <c r="AD92" s="16"/>
+      <c r="AE92" s="16"/>
+      <c r="AF92" s="16"/>
+      <c r="AG92" s="16"/>
+      <c r="AH92" s="16"/>
+      <c r="AI92" s="16"/>
+      <c r="AJ92" s="16"/>
+      <c r="AK92" s="16"/>
+      <c r="AL92" s="16"/>
+      <c r="AM92" s="16"/>
+      <c r="AN92" s="16"/>
+      <c r="AO92" s="16"/>
+      <c r="AP92" s="16"/>
+      <c r="AQ92" s="16"/>
+    </row>
+    <row r="93" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B93" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C70" s="4">
+      <c r="C93" s="4">
         <v>44677.82708333333</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D93" t="s">
         <v>202</v>
       </c>
-      <c r="E70" s="42" t="s">
+      <c r="E93" s="40" t="s">
         <v>201</v>
       </c>
-      <c r="F70" s="24" t="s">
+      <c r="F93" s="24" t="s">
         <v>200</v>
       </c>
+      <c r="G93" s="18"/>
+      <c r="H93" s="18"/>
+      <c r="I93" s="18"/>
+      <c r="J93" s="18"/>
+      <c r="K93" s="18"/>
+      <c r="L93" s="18"/>
+      <c r="M93" s="18"/>
+      <c r="N93" s="18"/>
+      <c r="O93" s="18"/>
+      <c r="P93" s="18"/>
+      <c r="Q93" s="18"/>
+      <c r="R93" s="18"/>
+      <c r="S93" s="18"/>
+      <c r="T93" s="18"/>
+      <c r="U93" s="18"/>
+      <c r="V93" s="18"/>
+      <c r="W93" s="18"/>
+      <c r="X93" s="18"/>
+      <c r="Y93" s="18"/>
+      <c r="Z93" s="16"/>
+      <c r="AA93" s="16"/>
+      <c r="AB93" s="16"/>
+      <c r="AC93" s="16"/>
+      <c r="AD93" s="16"/>
+      <c r="AE93" s="16"/>
+      <c r="AF93" s="16"/>
+      <c r="AG93" s="16"/>
+      <c r="AH93" s="16"/>
+      <c r="AI93" s="16"/>
+      <c r="AJ93" s="16"/>
+      <c r="AK93" s="16"/>
+      <c r="AL93" s="16"/>
+      <c r="AM93" s="16"/>
+      <c r="AN93" s="16"/>
+      <c r="AO93" s="16"/>
+      <c r="AP93" s="16"/>
+      <c r="AQ93" s="16"/>
+    </row>
+    <row r="94" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C94" t="s">
+        <v>280</v>
+      </c>
+      <c r="D94" t="s">
+        <v>281</v>
+      </c>
+      <c r="E94" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="F94" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="G94" s="18"/>
+      <c r="H94" s="18"/>
+      <c r="I94" s="18"/>
+      <c r="J94" s="18"/>
+      <c r="K94" s="18"/>
+      <c r="L94" s="18"/>
+      <c r="M94" s="18"/>
+      <c r="N94" s="18"/>
+      <c r="O94" s="18"/>
+      <c r="P94" s="18"/>
+      <c r="Q94" s="18"/>
+      <c r="R94" s="18"/>
+      <c r="S94" s="18"/>
+      <c r="T94" s="18"/>
+      <c r="U94" s="18"/>
+      <c r="V94" s="18"/>
+      <c r="W94" s="18"/>
+      <c r="X94" s="18"/>
+      <c r="Y94" s="18"/>
+      <c r="Z94" s="16"/>
+      <c r="AA94" s="16"/>
+      <c r="AB94" s="16"/>
+      <c r="AC94" s="16"/>
+      <c r="AD94" s="16"/>
+      <c r="AE94" s="16"/>
+      <c r="AF94" s="16"/>
+      <c r="AG94" s="16"/>
+      <c r="AH94" s="16"/>
+      <c r="AI94" s="16"/>
+      <c r="AJ94" s="16"/>
+      <c r="AK94" s="16"/>
+      <c r="AL94" s="16"/>
+      <c r="AM94" s="16"/>
+      <c r="AN94" s="16"/>
+      <c r="AO94" s="16"/>
+      <c r="AP94" s="16"/>
+      <c r="AQ94" s="16"/>
+    </row>
+    <row r="95" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="13"/>
+      <c r="B95" s="3"/>
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95" s="24"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="18"/>
+      <c r="I95" s="18"/>
+      <c r="J95" s="18"/>
+      <c r="K95" s="18"/>
+      <c r="L95" s="18"/>
+      <c r="M95" s="18"/>
+      <c r="N95" s="18"/>
+      <c r="O95" s="18"/>
+      <c r="P95" s="18"/>
+      <c r="Q95" s="18"/>
+      <c r="R95" s="18"/>
+      <c r="S95" s="18"/>
+      <c r="T95" s="18"/>
+      <c r="U95" s="18"/>
+      <c r="V95" s="18"/>
+      <c r="W95" s="18"/>
+      <c r="X95" s="18"/>
+      <c r="Y95" s="18"/>
+      <c r="Z95" s="16"/>
+      <c r="AA95" s="16"/>
+      <c r="AB95" s="16"/>
+      <c r="AC95" s="16"/>
+      <c r="AD95" s="16"/>
+      <c r="AE95" s="16"/>
+      <c r="AF95" s="16"/>
+      <c r="AG95" s="16"/>
+      <c r="AH95" s="16"/>
+      <c r="AI95" s="16"/>
+      <c r="AJ95" s="16"/>
+      <c r="AK95" s="16"/>
+      <c r="AL95" s="16"/>
+      <c r="AM95" s="16"/>
+      <c r="AN95" s="16"/>
+      <c r="AO95" s="16"/>
+      <c r="AP95" s="16"/>
+      <c r="AQ95" s="16"/>
+    </row>
+    <row r="100" spans="1:43" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="1:43" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A101" s="43">
+        <v>44682</v>
+      </c>
+      <c r="B101" s="43"/>
+      <c r="C101" s="43"/>
+      <c r="D101" s="43"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="22"/>
+    </row>
+    <row r="104" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="H104" s="46"/>
+    </row>
+    <row r="105" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="H105" s="46"/>
+    </row>
+    <row r="106" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="H106" s="46"/>
+    </row>
+    <row r="110" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="13"/>
+      <c r="B110" s="3"/>
+      <c r="C110"/>
+      <c r="D110"/>
+      <c r="E110"/>
+      <c r="F110" s="24"/>
+      <c r="G110" s="18"/>
+      <c r="H110" s="18"/>
+      <c r="I110" s="18"/>
+      <c r="J110" s="18"/>
+      <c r="K110" s="18"/>
+      <c r="L110" s="18"/>
+      <c r="M110" s="18"/>
+      <c r="N110" s="18"/>
+      <c r="O110" s="18"/>
+      <c r="P110" s="18"/>
+      <c r="Q110" s="18"/>
+      <c r="R110" s="18"/>
+      <c r="S110" s="18"/>
+      <c r="T110" s="18"/>
+      <c r="U110" s="18"/>
+      <c r="V110" s="18"/>
+      <c r="W110" s="18"/>
+      <c r="X110" s="18"/>
+      <c r="Y110" s="18"/>
+      <c r="Z110" s="16"/>
+      <c r="AA110" s="16"/>
+      <c r="AB110" s="16"/>
+      <c r="AC110" s="16"/>
+      <c r="AD110" s="16"/>
+      <c r="AE110" s="16"/>
+      <c r="AF110" s="16"/>
+      <c r="AG110" s="16"/>
+      <c r="AH110" s="16"/>
+      <c r="AI110" s="16"/>
+      <c r="AJ110" s="16"/>
+      <c r="AK110" s="16"/>
+      <c r="AL110" s="16"/>
+      <c r="AM110" s="16"/>
+      <c r="AN110" s="16"/>
+      <c r="AO110" s="16"/>
+      <c r="AP110" s="16"/>
+      <c r="AQ110" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A101:D101"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A2:D2"/>
@@ -3694,26 +5146,46 @@
     <hyperlink ref="B43" r:id="rId29"/>
     <hyperlink ref="I5" r:id="rId30"/>
     <hyperlink ref="B47" r:id="rId31"/>
-    <hyperlink ref="B48" r:id="rId32"/>
-    <hyperlink ref="B49" r:id="rId33" display="mailto:uddeshyas@chetu.com"/>
-    <hyperlink ref="B50" r:id="rId34" display="mailto:anupc@chetu.com"/>
-    <hyperlink ref="B51" r:id="rId35"/>
-    <hyperlink ref="B52" r:id="rId36"/>
-    <hyperlink ref="B53" r:id="rId37"/>
-    <hyperlink ref="B55" r:id="rId38"/>
-    <hyperlink ref="B56" r:id="rId39"/>
-    <hyperlink ref="B57" r:id="rId40"/>
-    <hyperlink ref="B60" r:id="rId41"/>
-    <hyperlink ref="B61" r:id="rId42"/>
-    <hyperlink ref="B58" r:id="rId43"/>
-    <hyperlink ref="B59" r:id="rId44"/>
-    <hyperlink ref="B70" r:id="rId45" display="mailto:anupc@chetu.com"/>
-    <hyperlink ref="B68" r:id="rId46" display="mailto:mayankr@chetu.com"/>
-    <hyperlink ref="B67" r:id="rId47" display="mailto:jyotid@chetu.com"/>
-    <hyperlink ref="B66" r:id="rId48" display="mailto:mayankr@chetu.com"/>
-    <hyperlink ref="B65" r:id="rId49" display="mailto:mayankr@chetu.com"/>
+    <hyperlink ref="B49" r:id="rId32"/>
+    <hyperlink ref="B50" r:id="rId33" display="mailto:uddeshyas@chetu.com"/>
+    <hyperlink ref="B51" r:id="rId34" display="mailto:anupc@chetu.com"/>
+    <hyperlink ref="B52" r:id="rId35"/>
+    <hyperlink ref="B53" r:id="rId36"/>
+    <hyperlink ref="B54" r:id="rId37"/>
+    <hyperlink ref="B56" r:id="rId38"/>
+    <hyperlink ref="B57" r:id="rId39"/>
+    <hyperlink ref="B58" r:id="rId40"/>
+    <hyperlink ref="B61" r:id="rId41"/>
+    <hyperlink ref="B62" r:id="rId42"/>
+    <hyperlink ref="B59" r:id="rId43"/>
+    <hyperlink ref="B60" r:id="rId44"/>
+    <hyperlink ref="B93" r:id="rId45" display="mailto:anupc@chetu.com"/>
+    <hyperlink ref="B91" r:id="rId46" display="mailto:mayankr@chetu.com"/>
+    <hyperlink ref="B90" r:id="rId47" display="mailto:jyotid@chetu.com"/>
+    <hyperlink ref="B89" r:id="rId48" display="mailto:mayankr@chetu.com"/>
+    <hyperlink ref="B88" r:id="rId49" display="mailto:mayankr@chetu.com"/>
+    <hyperlink ref="B86" r:id="rId50" display="mailto:jyotid@chetu.com"/>
+    <hyperlink ref="B85" r:id="rId51" display="mailto:anupc@chetu.com"/>
+    <hyperlink ref="B84" r:id="rId52" display="mailto:mayankr@chetu.com"/>
+    <hyperlink ref="B83" r:id="rId53" display="mailto:mayankr@chetu.com"/>
+    <hyperlink ref="B81" r:id="rId54" display="mailto:uddeshyas@chetu.com"/>
+    <hyperlink ref="B80" r:id="rId55" display="mailto:anupc@chetu.com"/>
+    <hyperlink ref="B79" r:id="rId56"/>
+    <hyperlink ref="B78" r:id="rId57" display="mailto:anupc@chetu.com"/>
+    <hyperlink ref="B77" r:id="rId58" display="mailto:gautamb@chetu.com"/>
+    <hyperlink ref="B76" r:id="rId59" display="mailto:anupc@chetu.com"/>
+    <hyperlink ref="B75" r:id="rId60"/>
+    <hyperlink ref="B74" r:id="rId61" display="mailto:junaidh@chetu.com"/>
+    <hyperlink ref="B73" r:id="rId62"/>
+    <hyperlink ref="B72" r:id="rId63" display="mailto:uddeshyas@chetu.com"/>
+    <hyperlink ref="B67" r:id="rId64"/>
+    <hyperlink ref="B66" r:id="rId65"/>
+    <hyperlink ref="B65" r:id="rId66" display="mailto:tarung@chetu.com"/>
+    <hyperlink ref="B63" r:id="rId67" display="mailto:jhalakk@chetu.com"/>
+    <hyperlink ref="B64" r:id="rId68" display="mailto:uddeshyas@chetu.com"/>
+    <hyperlink ref="B94" r:id="rId69" display="mailto:anupc@chetu.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId50"/>
+  <pageSetup orientation="portrait" r:id="rId70"/>
 </worksheet>
 </file>
</xml_diff>